<commit_message>
分支：dyt_targetApi31_0825 版本：VersionName:1.5.12 ,VersionCode:262 MTI448 版本 在芬兰语中显示app_name 为Pir的问题 上传时间：2023年1月31日15:20:47
</commit_message>
<xml_diff>
--- a/app/项目分支详情合表_外发.xlsx
+++ b/app/项目分支详情合表_外发.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" activeTab="1"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="SN区分表" sheetId="1" r:id="rId1"/>
@@ -1816,10 +1816,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1884,7 +1884,114 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1900,44 +2007,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1945,76 +2015,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2048,6 +2048,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2060,25 +2108,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2090,55 +2126,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2156,7 +2144,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2168,19 +2198,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2192,19 +2216,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2216,19 +2228,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2291,6 +2291,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -2329,17 +2344,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2358,35 +2387,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2395,10 +2395,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2407,133 +2407,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2942,8 +2942,8 @@
   <sheetPr/>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.75" customHeight="1"/>
@@ -3770,7 +3770,7 @@
   <sheetPr/>
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A48" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A41" workbookViewId="0">
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>

</xml_diff>